<commit_message>
Added data sources used in 2022 sales forecast ✔️
</commit_message>
<xml_diff>
--- a/2022-01-05/data/state_cannabis_data.xlsx
+++ b/2022-01-05/data/state_cannabis_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keega\Documents\cannlytics\cannabis-data-science\2022-01-05\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75ED6236-2383-46A9-B5EF-802CAF62E645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D77EC11-FA73-4CA4-8569-67CC2873E4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D718EB59-D1FB-4610-B646-AAC12D856547}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="85">
   <si>
     <t>state</t>
   </si>
@@ -55,12 +55,6 @@
     <t>https://mmcc.maryland.gov/Documents/Data%2c%20Stats%2c%20Resources%20Page%20Docs/Commission%20Stats/commision_stats_edibles_sales%28Nov2021%29.pdf</t>
   </si>
   <si>
-    <t>2021 Monthly Dispensary Edibles Sales</t>
-  </si>
-  <si>
-    <t>Flower Weight Sold by Growers (LBS)</t>
-  </si>
-  <si>
     <t>https://mmcc.maryland.gov/Documents/Data%2c%20Stats%2c%20Resources%20Page%20Docs/Commission%20Stats/commision_stats_flower_weight%28dec2021%29.pdf</t>
   </si>
   <si>
@@ -109,9 +103,6 @@
     <t>sales_per_retailer</t>
   </si>
   <si>
-    <t>Dispensary Sales</t>
-  </si>
-  <si>
     <t>total_retailers</t>
   </si>
   <si>
@@ -182,6 +173,123 @@
   </si>
   <si>
     <t>https://knowthefactsmmj.com/about/weekly-updates/</t>
+  </si>
+  <si>
+    <t>Maryland 2021 Monthly Dispensary Edibles Sales</t>
+  </si>
+  <si>
+    <t>Maryland Flower Weight Sold by Growers (LBS)</t>
+  </si>
+  <si>
+    <t>Maryland Vape Products</t>
+  </si>
+  <si>
+    <t>Maryland Patients</t>
+  </si>
+  <si>
+    <t>Maryland Dispensary Sales</t>
+  </si>
+  <si>
+    <t>Maryland Infused Products</t>
+  </si>
+  <si>
+    <t>Maryland Data</t>
+  </si>
+  <si>
+    <t>Illinois Licensed Adult Use Cannabis Dispensaries</t>
+  </si>
+  <si>
+    <t>https://www.idfpr.com/LicenseLookup/AdultUseDispensaries.pdf</t>
+  </si>
+  <si>
+    <t>Massachusetts Retail Sales by Date and Product Type</t>
+  </si>
+  <si>
+    <t>Massachusetts Average Monthly Price per Ounce for Adult-Use Cannabis</t>
+  </si>
+  <si>
+    <t>Massachusetts Plant Activity and Volume</t>
+  </si>
+  <si>
+    <t>https://dev.socrata.com/foundry/opendata.mass-cannabis-control.com/xwf2-j7g9</t>
+  </si>
+  <si>
+    <t>https://dev.socrata.com/foundry/opendata.mass-cannabis-control.com/hmwt-yiqy</t>
+  </si>
+  <si>
+    <t>https://dev.socrata.com/foundry/opendata.mass-cannabis-control.com/rqtv-uenj</t>
+  </si>
+  <si>
+    <t>https://dev.socrata.com/foundry/opendata.mass-cannabis-control.com/j3q7-3usu</t>
+  </si>
+  <si>
+    <t>https://dev.socrata.com/foundry/opendata.mass-cannabis-control.com/87rp-xn9v</t>
+  </si>
+  <si>
+    <t>https://www.idfpr.com/Forms/AUC/2021%2011%2002%20IDFPR%20monthly%20adult%20use%20cannabis%20sales.pdf</t>
+  </si>
+  <si>
+    <t>Washington Sales by Retailer by Month</t>
+  </si>
+  <si>
+    <t>https://lcb.wa.gov/sites/default/files/publications/Marijuana/sales_activity/2021-12-06-MJ-Sales-Activity-by-License-Number-Traceability-Contingency-Reporting-Retail.xlsx</t>
+  </si>
+  <si>
+    <t>https://lcb.app.box.com/s/e89t59s0yb558tjoncjsid710oirqbgd?page=1</t>
+  </si>
+  <si>
+    <t>Washington Traceability Data 2018 Through November 2021</t>
+  </si>
+  <si>
+    <t>Massachusetts Approved Licensees</t>
+  </si>
+  <si>
+    <t>Massachusetts Weekly Sales by Product Type</t>
+  </si>
+  <si>
+    <t>Illinois Adult Use Cannabis Monthly Sales Figures</t>
+  </si>
+  <si>
+    <t>U.S. Census Bureau, Resident Population in Colorado [COPOP], retrieved from FRED, Federal Reserve Bank of St. Louis</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/series/COPOP</t>
+  </si>
+  <si>
+    <t>U.S. Census Bureau, Resident Population in Washington [WAPOP], retrieved from FRED, Federal Reserve Bank of St. Louis</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/series/WAPOP</t>
+  </si>
+  <si>
+    <t>U.S. Census Bureau, Resident Population in Illinois [ILPOP], retrieved from FRED, Federal Reserve Bank of St. Louis</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/series/ILPOP</t>
+  </si>
+  <si>
+    <t>U.S. Census Bureau, Resident Population in Massachusetts [MAPOP], retrieved from FRED, Federal Reserve Bank of St. Louis</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/series/MAPOP</t>
+  </si>
+  <si>
+    <t>U.S. Census Bureau, Resident Population in Maine [MEPOP], retrieved from FRED, Federal Reserve Bank of St. Louis</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/series/MEPOP</t>
+  </si>
+  <si>
+    <t>U.S. Census Bureau, Resident Population in Maryland [MDPOP], retrieved from FRED, Federal Reserve Bank of St. Louis</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/series/MDPOP</t>
+  </si>
+  <si>
+    <t>U.S. Census Bureau, Resident Population in Oregon [ORPOP], retrieved from FRED, Federal Reserve Bank of St. Louis</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/series/ORPOP</t>
   </si>
 </sst>
 </file>
@@ -191,7 +299,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +311,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -255,10 +371,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -270,8 +387,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -588,7 +707,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -613,58 +732,58 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
@@ -672,7 +791,7 @@
         <v>41670</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2">
         <v>46563933</v>
@@ -686,7 +805,7 @@
         <v>41698</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C3">
         <v>45987045</v>
@@ -700,7 +819,7 @@
         <v>41729</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C4">
         <v>54703509</v>
@@ -714,7 +833,7 @@
         <v>41759</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C5">
         <v>53452855</v>
@@ -728,7 +847,7 @@
         <v>41790</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C6">
         <v>52730209</v>
@@ -742,7 +861,7 @@
         <v>41820</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C7">
         <v>53928391</v>
@@ -756,7 +875,7 @@
         <v>41851</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C8">
         <v>61004415</v>
@@ -770,7 +889,7 @@
         <v>41882</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C9">
         <v>67432834</v>
@@ -784,7 +903,7 @@
         <v>41912</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C10">
         <v>63066595</v>
@@ -798,7 +917,7 @@
         <v>41943</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C11">
         <v>62965201</v>
@@ -812,7 +931,7 @@
         <v>41973</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C12">
         <v>58448588</v>
@@ -826,7 +945,7 @@
         <v>42004</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C13">
         <v>63240164</v>
@@ -840,7 +959,7 @@
         <v>42035</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C14">
         <v>67405866</v>
@@ -854,7 +973,7 @@
         <v>42063</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C15">
         <v>64909262</v>
@@ -868,7 +987,7 @@
         <v>42094</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C16">
         <v>75773174</v>
@@ -882,7 +1001,7 @@
         <v>42124</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C17">
         <v>76711461</v>
@@ -896,7 +1015,7 @@
         <v>42155</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C18">
         <v>78199969</v>
@@ -910,7 +1029,7 @@
         <v>42185</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C19">
         <v>81012614</v>
@@ -924,7 +1043,7 @@
         <v>42216</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C20">
         <v>95926250</v>
@@ -938,7 +1057,7 @@
         <v>42247</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C21">
         <v>98498850</v>
@@ -952,7 +1071,7 @@
         <v>42277</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C22">
         <v>93631179</v>
@@ -966,7 +1085,7 @@
         <v>42308</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C23">
         <v>91210544</v>
@@ -980,7 +1099,7 @@
         <v>42338</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C24">
         <v>80224191</v>
@@ -994,7 +1113,7 @@
         <v>42369</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C25">
         <v>92087895</v>
@@ -1008,7 +1127,7 @@
         <v>42400</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C26">
         <v>88756562</v>
@@ -1022,7 +1141,7 @@
         <v>42429</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C27">
         <v>91064548</v>
@@ -1036,7 +1155,7 @@
         <v>42460</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C28">
         <v>103237561</v>
@@ -1050,7 +1169,7 @@
         <v>42490</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C29">
         <v>102135831</v>
@@ -1064,7 +1183,7 @@
         <v>42521</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C30">
         <v>101467366</v>
@@ -1078,7 +1197,7 @@
         <v>42551</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C31">
         <v>106059413</v>
@@ -1092,7 +1211,7 @@
         <v>42582</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C32">
         <v>121608432</v>
@@ -1106,7 +1225,7 @@
         <v>42613</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C33">
         <v>125112311</v>
@@ -1120,7 +1239,7 @@
         <v>42643</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C34">
         <v>125809892</v>
@@ -1134,7 +1253,7 @@
         <v>42674</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C35">
         <v>116635868</v>
@@ -1148,7 +1267,7 @@
         <v>42704</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C36">
         <v>109222331</v>
@@ -1162,7 +1281,7 @@
         <v>42735</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C37">
         <v>116093358</v>
@@ -1176,7 +1295,7 @@
         <v>42766</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C38">
         <v>107731031</v>
@@ -1190,7 +1309,7 @@
         <v>42794</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C39">
         <v>106740379</v>
@@ -1204,7 +1323,7 @@
         <v>42825</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C40">
         <v>130363830</v>
@@ -1218,7 +1337,7 @@
         <v>42855</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C41">
         <v>124272673</v>
@@ -1232,7 +1351,7 @@
         <v>42886</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C42">
         <v>123534419</v>
@@ -1246,7 +1365,7 @@
         <v>42916</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C43">
         <v>128951217</v>
@@ -1260,7 +1379,7 @@
         <v>42947</v>
       </c>
       <c r="B44" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C44">
         <v>136294447</v>
@@ -1274,7 +1393,7 @@
         <v>42978</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C45">
         <v>138469157</v>
@@ -1288,7 +1407,7 @@
         <v>43008</v>
       </c>
       <c r="B46" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C46">
         <v>135798669</v>
@@ -1302,7 +1421,7 @@
         <v>43039</v>
       </c>
       <c r="B47" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C47">
         <v>127706166</v>
@@ -1316,7 +1435,7 @@
         <v>43069</v>
       </c>
       <c r="B48" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C48">
         <v>119567777</v>
@@ -1330,7 +1449,7 @@
         <v>43100</v>
       </c>
       <c r="B49" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C49">
         <v>128272454</v>
@@ -1344,7 +1463,7 @@
         <v>43131</v>
       </c>
       <c r="B50" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C50">
         <v>117993222</v>
@@ -1358,7 +1477,7 @@
         <v>43159</v>
       </c>
       <c r="B51" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C51">
         <v>112509517</v>
@@ -1372,7 +1491,7 @@
         <v>43190</v>
       </c>
       <c r="B52" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C52">
         <v>135183956</v>
@@ -1386,7 +1505,7 @@
         <v>43220</v>
       </c>
       <c r="B53" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C53">
         <v>124309879</v>
@@ -1400,7 +1519,7 @@
         <v>43251</v>
       </c>
       <c r="B54" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C54">
         <v>122868216</v>
@@ -1414,7 +1533,7 @@
         <v>43281</v>
       </c>
       <c r="B55" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C55">
         <v>129523030</v>
@@ -1428,7 +1547,7 @@
         <v>43312</v>
       </c>
       <c r="B56" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C56">
         <v>138535584</v>
@@ -1442,7 +1561,7 @@
         <v>43343</v>
       </c>
       <c r="B57" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C57">
         <v>141322108</v>
@@ -1456,7 +1575,7 @@
         <v>43373</v>
       </c>
       <c r="B58" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C58">
         <v>135536453</v>
@@ -1470,7 +1589,7 @@
         <v>43404</v>
       </c>
       <c r="B59" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C59">
         <v>129224771</v>
@@ -1484,7 +1603,7 @@
         <v>43434</v>
       </c>
       <c r="B60" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C60">
         <v>123939891</v>
@@ -1498,7 +1617,7 @@
         <v>43465</v>
       </c>
       <c r="B61" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C61">
         <v>134744454</v>
@@ -1512,7 +1631,7 @@
         <v>43496</v>
       </c>
       <c r="B62" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C62">
         <v>124874274</v>
@@ -1526,7 +1645,7 @@
         <v>43524</v>
       </c>
       <c r="B63" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C63">
         <v>119407860</v>
@@ -1540,7 +1659,7 @@
         <v>43555</v>
       </c>
       <c r="B64" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C64">
         <v>142415604</v>
@@ -1554,7 +1673,7 @@
         <v>43585</v>
       </c>
       <c r="B65" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C65">
         <v>135882169</v>
@@ -1568,7 +1687,7 @@
         <v>43616</v>
       </c>
       <c r="B66" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C66">
         <v>143107279</v>
@@ -1582,7 +1701,7 @@
         <v>43646</v>
       </c>
       <c r="B67" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C67">
         <v>152026091</v>
@@ -1596,7 +1715,7 @@
         <v>43677</v>
       </c>
       <c r="B68" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C68">
         <v>166294715</v>
@@ -1610,7 +1729,7 @@
         <v>43708</v>
       </c>
       <c r="B69" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C69">
         <v>173219859</v>
@@ -1624,7 +1743,7 @@
         <v>43738</v>
       </c>
       <c r="B70" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C70">
         <v>155455167</v>
@@ -1638,7 +1757,7 @@
         <v>43769</v>
       </c>
       <c r="B71" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C71">
         <v>150476259</v>
@@ -1652,7 +1771,7 @@
         <v>43799</v>
       </c>
       <c r="B72" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C72">
         <v>141078975</v>
@@ -1666,7 +1785,7 @@
         <v>43830</v>
       </c>
       <c r="B73" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C73">
         <v>143752376</v>
@@ -1680,7 +1799,7 @@
         <v>43861</v>
       </c>
       <c r="B74" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C74">
         <v>139132265</v>
@@ -1694,7 +1813,7 @@
         <v>43890</v>
       </c>
       <c r="B75" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C75">
         <v>138626348</v>
@@ -1708,7 +1827,7 @@
         <v>43921</v>
       </c>
       <c r="B76" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C76">
         <v>161046706</v>
@@ -1722,7 +1841,7 @@
         <v>43951</v>
       </c>
       <c r="B77" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C77">
         <v>148495718</v>
@@ -1736,7 +1855,7 @@
         <v>43982</v>
       </c>
       <c r="B78" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C78">
         <v>192175937</v>
@@ -1750,7 +1869,7 @@
         <v>44012</v>
       </c>
       <c r="B79" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C79">
         <v>198873210</v>
@@ -1764,7 +1883,7 @@
         <v>44043</v>
       </c>
       <c r="B80" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C80">
         <v>226374568</v>
@@ -1778,7 +1897,7 @@
         <v>44074</v>
       </c>
       <c r="B81" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C81">
         <v>218601341</v>
@@ -1792,7 +1911,7 @@
         <v>44104</v>
       </c>
       <c r="B82" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C82">
         <v>206488268</v>
@@ -1806,7 +1925,7 @@
         <v>44135</v>
       </c>
       <c r="B83" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C83">
         <v>199788864</v>
@@ -1820,7 +1939,7 @@
         <v>44165</v>
       </c>
       <c r="B84" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C84">
         <v>175145246</v>
@@ -1834,7 +1953,7 @@
         <v>44196</v>
       </c>
       <c r="B85" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C85">
         <v>186343208</v>
@@ -1848,7 +1967,7 @@
         <v>44227</v>
       </c>
       <c r="B86" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C86">
         <v>187603697</v>
@@ -1862,7 +1981,7 @@
         <v>44255</v>
       </c>
       <c r="B87" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C87">
         <v>167037775</v>
@@ -1876,7 +1995,7 @@
         <v>44286</v>
       </c>
       <c r="B88" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C88">
         <v>207102063</v>
@@ -1890,7 +2009,7 @@
         <v>44316</v>
       </c>
       <c r="B89" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C89">
         <v>206324167</v>
@@ -1904,7 +2023,7 @@
         <v>44347</v>
       </c>
       <c r="B90" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C90">
         <v>157221754</v>
@@ -1918,7 +2037,7 @@
         <v>44377</v>
       </c>
       <c r="B91" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C91" s="6">
         <v>152719813</v>
@@ -1932,7 +2051,7 @@
         <v>44408</v>
       </c>
       <c r="B92" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C92">
         <v>167805366</v>
@@ -1946,7 +2065,7 @@
         <v>44439</v>
       </c>
       <c r="B93" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C93">
         <v>157994708</v>
@@ -1960,7 +2079,7 @@
         <v>44469</v>
       </c>
       <c r="B94" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C94">
         <v>150781653</v>
@@ -1974,7 +2093,7 @@
         <v>44500</v>
       </c>
       <c r="B95" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C95">
         <v>147137979</v>
@@ -1988,7 +2107,7 @@
         <v>43861</v>
       </c>
       <c r="B96" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C96">
         <v>39247840.829999998</v>
@@ -2017,7 +2136,7 @@
         <v>43890</v>
       </c>
       <c r="B97" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C97">
         <v>34805072.009999998</v>
@@ -2046,7 +2165,7 @@
         <v>43921</v>
       </c>
       <c r="B98" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C98">
         <v>35902543.219999999</v>
@@ -2075,7 +2194,7 @@
         <v>43951</v>
       </c>
       <c r="B99" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C99">
         <v>37260497.890000001</v>
@@ -2104,7 +2223,7 @@
         <v>43982</v>
       </c>
       <c r="B100" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C100">
         <v>44317385.719999999</v>
@@ -2133,7 +2252,7 @@
         <v>44012</v>
       </c>
       <c r="B101" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C101">
         <v>47646437.25</v>
@@ -2162,7 +2281,7 @@
         <v>44043</v>
       </c>
       <c r="B102" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C102">
         <v>60956981.409999996</v>
@@ -2191,7 +2310,7 @@
         <v>44074</v>
       </c>
       <c r="B103" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C103">
         <v>63963846.899999999</v>
@@ -2220,7 +2339,7 @@
         <v>44104</v>
       </c>
       <c r="B104" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C104">
         <v>67648362.140000001</v>
@@ -2249,7 +2368,7 @@
         <v>44135</v>
       </c>
       <c r="B105" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C105">
         <v>75278200.150000006</v>
@@ -2278,7 +2397,7 @@
         <v>44165</v>
       </c>
       <c r="B106" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C106">
         <v>75199344.329999998</v>
@@ -2307,7 +2426,7 @@
         <v>44196</v>
       </c>
       <c r="B107" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C107">
         <v>86857898.269999996</v>
@@ -2336,7 +2455,7 @@
         <v>44227</v>
       </c>
       <c r="B108" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C108">
         <v>88813872.780000001</v>
@@ -2365,7 +2484,7 @@
         <v>44255</v>
       </c>
       <c r="B109" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C109">
         <v>80741641.840000004</v>
@@ -2394,7 +2513,7 @@
         <v>44286</v>
       </c>
       <c r="B110" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C110">
         <v>109149355.98</v>
@@ -2423,7 +2542,7 @@
         <v>44316</v>
       </c>
       <c r="B111" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C111">
         <v>114961668.22</v>
@@ -2452,7 +2571,7 @@
         <v>44347</v>
       </c>
       <c r="B112" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C112">
         <v>116380348.01000001</v>
@@ -2481,7 +2600,7 @@
         <v>44377</v>
       </c>
       <c r="B113" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C113">
         <v>115574741.27</v>
@@ -2510,7 +2629,7 @@
         <v>44408</v>
       </c>
       <c r="B114" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C114">
         <v>127794220.5</v>
@@ -2539,7 +2658,7 @@
         <v>44439</v>
       </c>
       <c r="B115" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C115">
         <v>121933542.23</v>
@@ -2568,7 +2687,7 @@
         <v>44469</v>
       </c>
       <c r="B116" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C116">
         <v>121717709.51000001</v>
@@ -2597,7 +2716,7 @@
         <v>44500</v>
       </c>
       <c r="B117" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C117">
         <v>123375372.44</v>
@@ -2626,7 +2745,7 @@
         <v>43434</v>
       </c>
       <c r="B118" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C118">
         <v>3620367.69</v>
@@ -2648,7 +2767,7 @@
         <v>48.85</v>
       </c>
       <c r="J118" s="2">
-        <f>I118/3.5</f>
+        <f t="shared" ref="J118:J153" si="0">I118/3.5</f>
         <v>13.957142857142857</v>
       </c>
     </row>
@@ -2657,7 +2776,7 @@
         <v>43465</v>
       </c>
       <c r="B119" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C119">
         <v>12840334.4</v>
@@ -2678,7 +2797,7 @@
         <v>48.64</v>
       </c>
       <c r="J119" s="2">
-        <f>I119/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.897142857142857</v>
       </c>
     </row>
@@ -2687,7 +2806,7 @@
         <v>43496</v>
       </c>
       <c r="B120" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C120">
         <v>15604068.300000001</v>
@@ -2708,7 +2827,7 @@
         <v>50.05</v>
       </c>
       <c r="J120" s="2">
-        <f>I120/3.5</f>
+        <f t="shared" si="0"/>
         <v>14.299999999999999</v>
       </c>
     </row>
@@ -2717,7 +2836,7 @@
         <v>43524</v>
       </c>
       <c r="B121" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C121">
         <v>18190603.579999998</v>
@@ -2738,7 +2857,7 @@
         <v>50.63</v>
       </c>
       <c r="J121" s="2">
-        <f>I121/3.5</f>
+        <f t="shared" si="0"/>
         <v>14.465714285714286</v>
       </c>
     </row>
@@ -2747,7 +2866,7 @@
         <v>43555</v>
       </c>
       <c r="B122" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C122">
         <v>24362196.41</v>
@@ -2768,7 +2887,7 @@
         <v>50.45</v>
       </c>
       <c r="J122" s="2">
-        <f>I122/3.5</f>
+        <f t="shared" si="0"/>
         <v>14.414285714285715</v>
       </c>
     </row>
@@ -2777,7 +2896,7 @@
         <v>43585</v>
       </c>
       <c r="B123" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C123">
         <v>30771878.40000001</v>
@@ -2798,7 +2917,7 @@
         <v>48.74</v>
       </c>
       <c r="J123" s="2">
-        <f>I123/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.925714285714287</v>
       </c>
     </row>
@@ -2807,7 +2926,7 @@
         <v>43616</v>
       </c>
       <c r="B124" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C124">
         <v>36803203.99000001</v>
@@ -2828,7 +2947,7 @@
         <v>47.9</v>
       </c>
       <c r="J124" s="2">
-        <f>I124/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.685714285714285</v>
       </c>
     </row>
@@ -2837,7 +2956,7 @@
         <v>43646</v>
       </c>
       <c r="B125" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C125">
         <v>41455138.609999977</v>
@@ -2858,7 +2977,7 @@
         <v>47.12</v>
       </c>
       <c r="J125" s="2">
-        <f>I125/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.462857142857143</v>
       </c>
     </row>
@@ -2867,7 +2986,7 @@
         <v>43677</v>
       </c>
       <c r="B126" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C126">
         <v>45162637.439999998</v>
@@ -2888,7 +3007,7 @@
         <v>46.24</v>
       </c>
       <c r="J126" s="2">
-        <f>I126/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.211428571428572</v>
       </c>
     </row>
@@ -2897,7 +3016,7 @@
         <v>43708</v>
       </c>
       <c r="B127" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C127">
         <v>49247203.150000043</v>
@@ -2918,7 +3037,7 @@
         <v>46.46</v>
       </c>
       <c r="J127" s="2">
-        <f>I127/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.274285714285714</v>
       </c>
     </row>
@@ -2927,7 +3046,7 @@
         <v>43738</v>
       </c>
       <c r="B128" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C128">
         <v>45230052.289999962</v>
@@ -2948,7 +3067,7 @@
         <v>46.56</v>
       </c>
       <c r="J128" s="2">
-        <f>I128/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.302857142857144</v>
       </c>
     </row>
@@ -2957,7 +3076,7 @@
         <v>43769</v>
       </c>
       <c r="B129" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C129">
         <v>42740057.569999993</v>
@@ -2978,7 +3097,7 @@
         <v>47.78</v>
       </c>
       <c r="J129" s="2">
-        <f>I129/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.651428571428571</v>
       </c>
     </row>
@@ -2987,7 +3106,7 @@
         <v>43799</v>
       </c>
       <c r="B130" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C130">
         <v>45788156.810000002</v>
@@ -3008,7 +3127,7 @@
         <v>47.93</v>
       </c>
       <c r="J130" s="2">
-        <f>I130/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.694285714285714</v>
       </c>
     </row>
@@ -3017,7 +3136,7 @@
         <v>43830</v>
       </c>
       <c r="B131" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C131">
         <v>49748353.530000031</v>
@@ -3038,7 +3157,7 @@
         <v>47.85</v>
       </c>
       <c r="J131" s="2">
-        <f>I131/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.671428571428573</v>
       </c>
     </row>
@@ -3047,7 +3166,7 @@
         <v>43861</v>
       </c>
       <c r="B132" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C132">
         <v>51839256.779999971</v>
@@ -3068,7 +3187,7 @@
         <v>48.01</v>
       </c>
       <c r="J132" s="2">
-        <f>I132/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.717142857142857</v>
       </c>
     </row>
@@ -3077,7 +3196,7 @@
         <v>43890</v>
       </c>
       <c r="B133" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C133">
         <v>55318610.370000057</v>
@@ -3098,7 +3217,7 @@
         <v>48.02</v>
       </c>
       <c r="J133" s="2">
-        <f>I133/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.72</v>
       </c>
     </row>
@@ -3107,7 +3226,7 @@
         <v>43921</v>
       </c>
       <c r="B134" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C134">
         <v>50269640.699999928</v>
@@ -3128,7 +3247,7 @@
         <v>45.3</v>
       </c>
       <c r="J134" s="2">
-        <f>I134/3.5</f>
+        <f t="shared" si="0"/>
         <v>12.942857142857141</v>
       </c>
     </row>
@@ -3137,7 +3256,7 @@
         <v>43951</v>
       </c>
       <c r="B135" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -3158,7 +3277,7 @@
         <v>37.380000000000003</v>
       </c>
       <c r="J135" s="2">
-        <f>I135/3.5</f>
+        <f t="shared" si="0"/>
         <v>10.680000000000001</v>
       </c>
     </row>
@@ -3167,7 +3286,7 @@
         <v>43982</v>
       </c>
       <c r="B136" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C136">
         <v>13551652.55000007</v>
@@ -3188,7 +3307,7 @@
         <v>40.04</v>
       </c>
       <c r="J136" s="2">
-        <f>I136/3.5</f>
+        <f t="shared" si="0"/>
         <v>11.44</v>
       </c>
     </row>
@@ -3197,7 +3316,7 @@
         <v>44012</v>
       </c>
       <c r="B137" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C137">
         <v>54657556.109999903</v>
@@ -3218,7 +3337,7 @@
         <v>46.39</v>
       </c>
       <c r="J137" s="2">
-        <f>I137/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.254285714285714</v>
       </c>
     </row>
@@ -3227,7 +3346,7 @@
         <v>44043</v>
       </c>
       <c r="B138" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C138">
         <v>72967506.920000076</v>
@@ -3248,7 +3367,7 @@
         <v>46.93</v>
       </c>
       <c r="J138" s="2">
-        <f>I138/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.408571428571429</v>
       </c>
     </row>
@@ -3257,7 +3376,7 @@
         <v>44074</v>
       </c>
       <c r="B139" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C139">
         <v>80310583.399999976</v>
@@ -3278,7 +3397,7 @@
         <v>47.37</v>
       </c>
       <c r="J139" s="2">
-        <f>I139/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.534285714285714</v>
       </c>
     </row>
@@ -3287,7 +3406,7 @@
         <v>44104</v>
       </c>
       <c r="B140" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C140">
         <v>79829846.99000001</v>
@@ -3308,7 +3427,7 @@
         <v>47.17</v>
       </c>
       <c r="J140" s="2">
-        <f>I140/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.477142857142857</v>
       </c>
     </row>
@@ -3317,7 +3436,7 @@
         <v>44135</v>
       </c>
       <c r="B141" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C141">
         <v>83362631.360000014</v>
@@ -3338,7 +3457,7 @@
         <v>47.38</v>
       </c>
       <c r="J141" s="2">
-        <f>I141/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.537142857142857</v>
       </c>
     </row>
@@ -3347,7 +3466,7 @@
         <v>44165</v>
       </c>
       <c r="B142" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C142">
         <v>76248701.070000052</v>
@@ -3368,7 +3487,7 @@
         <v>46.82</v>
       </c>
       <c r="J142" s="2">
-        <f>I142/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.377142857142857</v>
       </c>
     </row>
@@ -3377,7 +3496,7 @@
         <v>44196</v>
       </c>
       <c r="B143" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C143">
         <v>78439686.579999924</v>
@@ -3398,7 +3517,7 @@
         <v>46.44</v>
       </c>
       <c r="J143" s="2">
-        <f>I143/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.268571428571429</v>
       </c>
     </row>
@@ -3407,7 +3526,7 @@
         <v>44227</v>
       </c>
       <c r="B144" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C144">
         <v>31607705.050000191</v>
@@ -3428,7 +3547,7 @@
         <v>46.73</v>
       </c>
       <c r="J144" s="2">
-        <f>I144/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.351428571428571</v>
       </c>
     </row>
@@ -3437,7 +3556,7 @@
         <v>44255</v>
       </c>
       <c r="B145" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C145">
         <v>37371809.960000038</v>
@@ -3458,7 +3577,7 @@
         <v>46.75</v>
       </c>
       <c r="J145" s="2">
-        <f>I145/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.357142857142858</v>
       </c>
     </row>
@@ -3467,7 +3586,7 @@
         <v>44286</v>
       </c>
       <c r="B146" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C146">
         <v>76510082.049999952</v>
@@ -3488,7 +3607,7 @@
         <v>46.87</v>
       </c>
       <c r="J146" s="2">
-        <f>I146/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.391428571428571</v>
       </c>
     </row>
@@ -3497,7 +3616,7 @@
         <v>44316</v>
       </c>
       <c r="B147" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C147">
         <v>103155391.72</v>
@@ -3518,7 +3637,7 @@
         <v>46.38</v>
       </c>
       <c r="J147" s="2">
-        <f>I147/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.251428571428573</v>
       </c>
     </row>
@@ -3527,7 +3646,7 @@
         <v>44347</v>
       </c>
       <c r="B148" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C148">
         <v>110740748.47</v>
@@ -3548,7 +3667,7 @@
         <v>46.53</v>
       </c>
       <c r="J148" s="2">
-        <f>I148/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.294285714285715</v>
       </c>
     </row>
@@ -3557,7 +3676,7 @@
         <v>44377</v>
       </c>
       <c r="B149" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C149">
         <v>110267748.92000011</v>
@@ -3578,7 +3697,7 @@
         <v>46.15</v>
       </c>
       <c r="J149" s="2">
-        <f>I149/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.185714285714285</v>
       </c>
     </row>
@@ -3587,7 +3706,7 @@
         <v>44408</v>
       </c>
       <c r="B150" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C150">
         <v>119816430.6099999</v>
@@ -3608,7 +3727,7 @@
         <v>46.37</v>
       </c>
       <c r="J150" s="2">
-        <f>I150/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.248571428571427</v>
       </c>
     </row>
@@ -3617,7 +3736,7 @@
         <v>44439</v>
       </c>
       <c r="B151" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C151">
         <v>108935873.20999999</v>
@@ -3638,7 +3757,7 @@
         <v>45.88</v>
       </c>
       <c r="J151" s="2">
-        <f>I151/3.5</f>
+        <f t="shared" si="0"/>
         <v>13.108571428571429</v>
       </c>
     </row>
@@ -3647,7 +3766,7 @@
         <v>44469</v>
       </c>
       <c r="B152" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C152">
         <v>108402974.48999999</v>
@@ -3668,7 +3787,7 @@
         <v>45.31</v>
       </c>
       <c r="J152" s="2">
-        <f>I152/3.5</f>
+        <f t="shared" si="0"/>
         <v>12.945714285714287</v>
       </c>
     </row>
@@ -3677,7 +3796,7 @@
         <v>44500</v>
       </c>
       <c r="B153" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C153">
         <v>114702283.23</v>
@@ -3698,7 +3817,7 @@
         <v>44.83</v>
       </c>
       <c r="J153" s="2">
-        <f>I153/3.5</f>
+        <f t="shared" si="0"/>
         <v>12.808571428571428</v>
       </c>
     </row>
@@ -3707,7 +3826,7 @@
         <v>44530</v>
       </c>
       <c r="B154" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C154">
         <v>76099922.440000057</v>
@@ -3730,7 +3849,7 @@
         <v>44561</v>
       </c>
       <c r="B155" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C155">
         <v>51521329.929999828</v>
@@ -4078,7 +4197,7 @@
         <v>44196</v>
       </c>
       <c r="B169" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C169">
         <v>1920712.2</v>
@@ -4087,7 +4206,7 @@
         <v>1362280</v>
       </c>
       <c r="I169">
-        <f>J169*3.5</f>
+        <f t="shared" ref="I169:I200" si="1">J169*3.5</f>
         <v>52.884999999999998</v>
       </c>
       <c r="J169">
@@ -4099,7 +4218,7 @@
         <v>44227</v>
       </c>
       <c r="B170" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C170">
         <v>2470502.0299999998</v>
@@ -4108,7 +4227,7 @@
         <v>1372247</v>
       </c>
       <c r="I170">
-        <f>J170*3.5</f>
+        <f t="shared" si="1"/>
         <v>50.925000000000004</v>
       </c>
       <c r="J170">
@@ -4120,7 +4239,7 @@
         <v>44255</v>
       </c>
       <c r="B171" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C171">
         <v>2552394.14</v>
@@ -4129,7 +4248,7 @@
         <v>1372247</v>
       </c>
       <c r="I171">
-        <f>J171*3.5</f>
+        <f t="shared" si="1"/>
         <v>50.294999999999995</v>
       </c>
       <c r="J171">
@@ -4141,7 +4260,7 @@
         <v>44286</v>
       </c>
       <c r="B172" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C172">
         <v>3751561.54</v>
@@ -4150,7 +4269,7 @@
         <v>1372247</v>
       </c>
       <c r="I172">
-        <f>J172*3.5</f>
+        <f t="shared" si="1"/>
         <v>50.47</v>
       </c>
       <c r="J172">
@@ -4162,7 +4281,7 @@
         <v>44316</v>
       </c>
       <c r="B173" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C173">
         <v>4356087.5</v>
@@ -4171,7 +4290,7 @@
         <v>1372247</v>
       </c>
       <c r="I173">
-        <f>J173*3.5</f>
+        <f t="shared" si="1"/>
         <v>47.914999999999999</v>
       </c>
       <c r="J173">
@@ -4183,7 +4302,7 @@
         <v>44347</v>
       </c>
       <c r="B174" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C174">
         <v>5364958.05</v>
@@ -4192,7 +4311,7 @@
         <v>1372247</v>
       </c>
       <c r="I174">
-        <f>J174*3.5</f>
+        <f t="shared" si="1"/>
         <v>46.27</v>
       </c>
       <c r="J174">
@@ -4204,7 +4323,7 @@
         <v>44377</v>
       </c>
       <c r="B175" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C175">
         <v>6470807.0300000003</v>
@@ -4213,7 +4332,7 @@
         <v>1372247</v>
       </c>
       <c r="I175">
-        <f>J175*3.5</f>
+        <f t="shared" si="1"/>
         <v>46.199999999999996</v>
       </c>
       <c r="J175">
@@ -4225,7 +4344,7 @@
         <v>44408</v>
       </c>
       <c r="B176" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C176">
         <v>9452535.4499999993</v>
@@ -4234,7 +4353,7 @@
         <v>1372247</v>
       </c>
       <c r="I176">
-        <f>J176*3.5</f>
+        <f t="shared" si="1"/>
         <v>45.15</v>
       </c>
       <c r="J176">
@@ -4246,7 +4365,7 @@
         <v>44439</v>
       </c>
       <c r="B177" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C177">
         <v>10123444.5</v>
@@ -4255,7 +4374,7 @@
         <v>1372247</v>
       </c>
       <c r="I177">
-        <f>J177*3.5</f>
+        <f t="shared" si="1"/>
         <v>45.01</v>
       </c>
       <c r="J177">
@@ -4267,7 +4386,7 @@
         <v>44469</v>
       </c>
       <c r="B178" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C178">
         <v>9766861.5700000003</v>
@@ -4276,7 +4395,7 @@
         <v>1372247</v>
       </c>
       <c r="I178">
-        <f>J178*3.5</f>
+        <f t="shared" si="1"/>
         <v>43.645000000000003</v>
       </c>
       <c r="J178">
@@ -4288,7 +4407,7 @@
         <v>44500</v>
       </c>
       <c r="B179" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C179">
         <v>9507728.4100000001</v>
@@ -4297,7 +4416,7 @@
         <v>1372247</v>
       </c>
       <c r="I179">
-        <f>J179*3.5</f>
+        <f t="shared" si="1"/>
         <v>42.699999999999996</v>
       </c>
       <c r="J179">
@@ -4309,7 +4428,7 @@
         <v>44530</v>
       </c>
       <c r="B180" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C180">
         <v>8359845.5199999996</v>
@@ -4318,7 +4437,7 @@
         <v>1372247</v>
       </c>
       <c r="I180">
-        <f>J180*3.5</f>
+        <f t="shared" si="1"/>
         <v>41.51</v>
       </c>
       <c r="J180">
@@ -4330,7 +4449,7 @@
         <v>42674</v>
       </c>
       <c r="B181" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C181">
         <v>2542720.7599999998</v>
@@ -4339,7 +4458,7 @@
         <v>4093271</v>
       </c>
       <c r="I181">
-        <f>J181*3.5</f>
+        <f t="shared" si="1"/>
         <v>36.75</v>
       </c>
       <c r="J181">
@@ -4354,7 +4473,7 @@
         <v>42704</v>
       </c>
       <c r="B182" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C182">
         <v>4495401.2</v>
@@ -4363,7 +4482,7 @@
         <v>4093271</v>
       </c>
       <c r="I182">
-        <f>J182*3.5</f>
+        <f t="shared" si="1"/>
         <v>33.6</v>
       </c>
       <c r="J182">
@@ -4378,7 +4497,7 @@
         <v>42735</v>
       </c>
       <c r="B183" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C183">
         <v>7358744.9100000001</v>
@@ -4387,7 +4506,7 @@
         <v>4093271</v>
       </c>
       <c r="I183">
-        <f>J183*3.5</f>
+        <f t="shared" si="1"/>
         <v>31.5</v>
       </c>
       <c r="J183">
@@ -4405,7 +4524,7 @@
         <v>42766</v>
       </c>
       <c r="B184" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C184">
         <v>30505016.239999998</v>
@@ -4414,7 +4533,7 @@
         <v>4147294</v>
       </c>
       <c r="I184">
-        <f>J184*3.5</f>
+        <f t="shared" si="1"/>
         <v>30.625</v>
       </c>
       <c r="J184">
@@ -4432,7 +4551,7 @@
         <v>42794</v>
       </c>
       <c r="B185" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C185">
         <v>33304295.210000001</v>
@@ -4441,7 +4560,7 @@
         <v>4147294</v>
       </c>
       <c r="I185">
-        <f>J185*3.5</f>
+        <f t="shared" si="1"/>
         <v>29.925000000000004</v>
       </c>
       <c r="J185">
@@ -4459,7 +4578,7 @@
         <v>42825</v>
       </c>
       <c r="B186" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C186">
         <v>40167570.579999998</v>
@@ -4468,7 +4587,7 @@
         <v>4147294</v>
       </c>
       <c r="I186">
-        <f>J186*3.5</f>
+        <f t="shared" si="1"/>
         <v>29.82</v>
       </c>
       <c r="J186">
@@ -4486,7 +4605,7 @@
         <v>42855</v>
       </c>
       <c r="B187" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C187">
         <v>41221222.100000001</v>
@@ -4495,7 +4614,7 @@
         <v>4147294</v>
       </c>
       <c r="I187">
-        <f>J187*3.5</f>
+        <f t="shared" si="1"/>
         <v>29.155000000000001</v>
       </c>
       <c r="J187">
@@ -4513,7 +4632,7 @@
         <v>42886</v>
       </c>
       <c r="B188" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C188">
         <v>42821237.979999997</v>
@@ -4522,7 +4641,7 @@
         <v>4147294</v>
       </c>
       <c r="I188">
-        <f>J188*3.5</f>
+        <f t="shared" si="1"/>
         <v>29.155000000000001</v>
       </c>
       <c r="J188">
@@ -4540,7 +4659,7 @@
         <v>42916</v>
       </c>
       <c r="B189" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C189">
         <v>45142658.490000002</v>
@@ -4549,7 +4668,7 @@
         <v>4147294</v>
       </c>
       <c r="I189">
-        <f>J189*3.5</f>
+        <f t="shared" si="1"/>
         <v>28.735000000000003</v>
       </c>
       <c r="J189">
@@ -4567,7 +4686,7 @@
         <v>42947</v>
       </c>
       <c r="B190" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C190">
         <v>48594620.329999901</v>
@@ -4576,7 +4695,7 @@
         <v>4147294</v>
       </c>
       <c r="I190">
-        <f>J190*3.5</f>
+        <f t="shared" si="1"/>
         <v>28.349999999999998</v>
       </c>
       <c r="J190">
@@ -4594,7 +4713,7 @@
         <v>42978</v>
       </c>
       <c r="B191" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C191">
         <v>52291580.539999999</v>
@@ -4603,7 +4722,7 @@
         <v>4147294</v>
       </c>
       <c r="I191">
-        <f>J191*3.5</f>
+        <f t="shared" si="1"/>
         <v>28.770000000000003</v>
       </c>
       <c r="J191">
@@ -4621,7 +4740,7 @@
         <v>43008</v>
       </c>
       <c r="B192" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C192">
         <v>51031586.789999999</v>
@@ -4630,7 +4749,7 @@
         <v>4147294</v>
       </c>
       <c r="I192">
-        <f>J192*3.5</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="J192">
@@ -4648,7 +4767,7 @@
         <v>43039</v>
       </c>
       <c r="B193" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C193">
         <v>47006851.170000002</v>
@@ -4657,7 +4776,7 @@
         <v>4147294</v>
       </c>
       <c r="I193">
-        <f>J193*3.5</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="J193">
@@ -4675,7 +4794,7 @@
         <v>43069</v>
       </c>
       <c r="B194" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C194">
         <v>43487768.479999997</v>
@@ -4684,7 +4803,7 @@
         <v>4147294</v>
       </c>
       <c r="I194">
-        <f>J194*3.5</f>
+        <f t="shared" si="1"/>
         <v>25.795000000000002</v>
       </c>
       <c r="J194">
@@ -4702,7 +4821,7 @@
         <v>43100</v>
       </c>
       <c r="B195" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C195">
         <v>46778274.280000001</v>
@@ -4711,7 +4830,7 @@
         <v>4147294</v>
       </c>
       <c r="I195">
-        <f>J195*3.5</f>
+        <f t="shared" si="1"/>
         <v>24.535</v>
       </c>
       <c r="J195">
@@ -4729,7 +4848,7 @@
         <v>43131</v>
       </c>
       <c r="B196" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C196">
         <v>44569195.570000097</v>
@@ -4738,7 +4857,7 @@
         <v>4183538</v>
       </c>
       <c r="I196">
-        <f>J196*3.5</f>
+        <f t="shared" si="1"/>
         <v>23.344999999999999</v>
       </c>
       <c r="J196">
@@ -4756,7 +4875,7 @@
         <v>43159</v>
       </c>
       <c r="B197" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C197">
         <v>44973348.870000102</v>
@@ -4765,7 +4884,7 @@
         <v>4183538</v>
       </c>
       <c r="I197">
-        <f>J197*3.5</f>
+        <f t="shared" si="1"/>
         <v>22.295000000000002</v>
       </c>
       <c r="J197">
@@ -4783,7 +4902,7 @@
         <v>43190</v>
       </c>
       <c r="B198" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C198">
         <v>53032956.509999998</v>
@@ -4792,7 +4911,7 @@
         <v>4183538</v>
       </c>
       <c r="I198">
-        <f>J198*3.5</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="J198">
@@ -4810,7 +4929,7 @@
         <v>43220</v>
       </c>
       <c r="B199" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C199">
         <v>52493380.859999999</v>
@@ -4819,7 +4938,7 @@
         <v>4183538</v>
       </c>
       <c r="I199">
-        <f>J199*3.5</f>
+        <f t="shared" si="1"/>
         <v>19.810000000000002</v>
       </c>
       <c r="J199">
@@ -4837,7 +4956,7 @@
         <v>43251</v>
       </c>
       <c r="B200" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C200">
         <v>53872674.509999998</v>
@@ -4846,7 +4965,7 @@
         <v>4183538</v>
       </c>
       <c r="I200">
-        <f>J200*3.5</f>
+        <f t="shared" si="1"/>
         <v>20.3</v>
       </c>
       <c r="J200">
@@ -4864,7 +4983,7 @@
         <v>43281</v>
       </c>
       <c r="B201" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C201">
         <v>56138521.2999999</v>
@@ -4873,7 +4992,7 @@
         <v>4183538</v>
       </c>
       <c r="I201">
-        <f>J201*3.5</f>
+        <f t="shared" ref="I201:I232" si="2">J201*3.5</f>
         <v>19.459999999999997</v>
       </c>
       <c r="J201">
@@ -4891,7 +5010,7 @@
         <v>43312</v>
       </c>
       <c r="B202" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C202">
         <v>58183325.2999999</v>
@@ -4900,7 +5019,7 @@
         <v>4183538</v>
       </c>
       <c r="I202">
-        <f>J202*3.5</f>
+        <f t="shared" si="2"/>
         <v>18.55</v>
       </c>
       <c r="J202">
@@ -4918,7 +5037,7 @@
         <v>43343</v>
       </c>
       <c r="B203" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C203">
         <v>61433920.229999997</v>
@@ -4927,7 +5046,7 @@
         <v>4183538</v>
       </c>
       <c r="I203">
-        <f>J203*3.5</f>
+        <f t="shared" si="2"/>
         <v>17.920000000000002</v>
       </c>
       <c r="J203">
@@ -4945,7 +5064,7 @@
         <v>43373</v>
       </c>
       <c r="B204" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C204">
         <v>57604337.799999997</v>
@@ -4954,7 +5073,7 @@
         <v>4183538</v>
       </c>
       <c r="I204">
-        <f>J204*3.5</f>
+        <f t="shared" si="2"/>
         <v>17.5</v>
       </c>
       <c r="J204">
@@ -4972,7 +5091,7 @@
         <v>43404</v>
       </c>
       <c r="B205" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C205">
         <v>56114367.549999997</v>
@@ -4981,7 +5100,7 @@
         <v>4183538</v>
       </c>
       <c r="I205">
-        <f>J205*3.5</f>
+        <f t="shared" si="2"/>
         <v>17.5</v>
       </c>
       <c r="J205">
@@ -4999,7 +5118,7 @@
         <v>43434</v>
       </c>
       <c r="B206" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C206">
         <v>53752068.390000001</v>
@@ -5008,7 +5127,7 @@
         <v>4183538</v>
       </c>
       <c r="I206">
-        <f>J206*3.5</f>
+        <f t="shared" si="2"/>
         <v>16.8</v>
       </c>
       <c r="J206">
@@ -5026,7 +5145,7 @@
         <v>43465</v>
       </c>
       <c r="B207" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C207">
         <v>56224338.140000001</v>
@@ -5035,7 +5154,7 @@
         <v>4183538</v>
       </c>
       <c r="I207">
-        <f>J207*3.5</f>
+        <f t="shared" si="2"/>
         <v>16.66</v>
       </c>
       <c r="J207">
@@ -5053,7 +5172,7 @@
         <v>43496</v>
       </c>
       <c r="B208" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C208">
         <v>54280992.310000002</v>
@@ -5062,7 +5181,7 @@
         <v>4216116</v>
       </c>
       <c r="I208">
-        <f>J208*3.5</f>
+        <f t="shared" si="2"/>
         <v>15.924999999999999</v>
       </c>
       <c r="J208">
@@ -5080,7 +5199,7 @@
         <v>43524</v>
       </c>
       <c r="B209" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C209">
         <v>52773889.659999996</v>
@@ -5089,7 +5208,7 @@
         <v>4216116</v>
       </c>
       <c r="I209">
-        <f>J209*3.5</f>
+        <f t="shared" si="2"/>
         <v>15.015000000000001</v>
       </c>
       <c r="J209">
@@ -5107,7 +5226,7 @@
         <v>43555</v>
       </c>
       <c r="B210" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C210">
         <v>62119814.93</v>
@@ -5116,7 +5235,7 @@
         <v>4216116</v>
       </c>
       <c r="I210">
-        <f>J210*3.5</f>
+        <f t="shared" si="2"/>
         <v>14.944999999999999</v>
       </c>
       <c r="J210">
@@ -5134,7 +5253,7 @@
         <v>43585</v>
       </c>
       <c r="B211" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C211">
         <v>62369873.760000102</v>
@@ -5143,7 +5262,7 @@
         <v>4216116</v>
       </c>
       <c r="I211">
-        <f>J211*3.5</f>
+        <f t="shared" si="2"/>
         <v>14.594999999999999</v>
       </c>
       <c r="J211">
@@ -5161,7 +5280,7 @@
         <v>43616</v>
       </c>
       <c r="B212" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C212">
         <v>64574747.520000003</v>
@@ -5170,7 +5289,7 @@
         <v>4216116</v>
       </c>
       <c r="I212">
-        <f>J212*3.5</f>
+        <f t="shared" si="2"/>
         <v>14.665000000000001</v>
       </c>
       <c r="J212">
@@ -5188,7 +5307,7 @@
         <v>43646</v>
       </c>
       <c r="B213" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C213">
         <v>66593082.789999999</v>
@@ -5197,7 +5316,7 @@
         <v>4216116</v>
       </c>
       <c r="I213">
-        <f>J213*3.5</f>
+        <f t="shared" si="2"/>
         <v>15.015000000000001</v>
       </c>
       <c r="J213">
@@ -5215,7 +5334,7 @@
         <v>43677</v>
       </c>
       <c r="B214" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C214">
         <v>73144531.399999902</v>
@@ -5224,7 +5343,7 @@
         <v>4216116</v>
       </c>
       <c r="I214">
-        <f>J214*3.5</f>
+        <f t="shared" si="2"/>
         <v>16.52</v>
       </c>
       <c r="J214">
@@ -5242,7 +5361,7 @@
         <v>43708</v>
       </c>
       <c r="B215" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C215">
         <v>79371526.469999999</v>
@@ -5251,7 +5370,7 @@
         <v>4216116</v>
       </c>
       <c r="I215">
-        <f>J215*3.5</f>
+        <f t="shared" si="2"/>
         <v>17.5</v>
       </c>
       <c r="J215">
@@ -5269,7 +5388,7 @@
         <v>43738</v>
       </c>
       <c r="B216" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C216">
         <v>71611294.570000097</v>
@@ -5278,7 +5397,7 @@
         <v>4216116</v>
       </c>
       <c r="I216">
-        <f>J216*3.5</f>
+        <f t="shared" si="2"/>
         <v>17.5</v>
       </c>
       <c r="J216">
@@ -5296,7 +5415,7 @@
         <v>43769</v>
       </c>
       <c r="B217" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C217">
         <v>70857737.060000002</v>
@@ -5305,7 +5424,7 @@
         <v>4216116</v>
       </c>
       <c r="I217">
-        <f>J217*3.5</f>
+        <f t="shared" si="2"/>
         <v>17.535</v>
       </c>
       <c r="J217">
@@ -5323,7 +5442,7 @@
         <v>43799</v>
       </c>
       <c r="B218" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C218">
         <v>68507652.840000004</v>
@@ -5332,7 +5451,7 @@
         <v>4216116</v>
       </c>
       <c r="I218">
-        <f>J218*3.5</f>
+        <f t="shared" si="2"/>
         <v>18.2</v>
       </c>
       <c r="J218">
@@ -5350,7 +5469,7 @@
         <v>43830</v>
       </c>
       <c r="B219" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C219">
         <v>68928674.280000001</v>
@@ -5359,7 +5478,7 @@
         <v>4216116</v>
       </c>
       <c r="I219">
-        <f>J219*3.5</f>
+        <f t="shared" si="2"/>
         <v>17.5</v>
       </c>
       <c r="J219">
@@ -5377,7 +5496,7 @@
         <v>43861</v>
       </c>
       <c r="B220" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C220">
         <v>68653599.900000006</v>
@@ -5386,7 +5505,7 @@
         <v>4241507</v>
       </c>
       <c r="I220">
-        <f>J220*3.5</f>
+        <f t="shared" si="2"/>
         <v>17.5</v>
       </c>
       <c r="J220">
@@ -5404,7 +5523,7 @@
         <v>43890</v>
       </c>
       <c r="B221" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C221">
         <v>69788785.580000103</v>
@@ -5413,7 +5532,7 @@
         <v>4241507</v>
       </c>
       <c r="I221">
-        <f>J221*3.5</f>
+        <f t="shared" si="2"/>
         <v>17.5</v>
       </c>
       <c r="J221">
@@ -5431,7 +5550,7 @@
         <v>43921</v>
       </c>
       <c r="B222" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C222">
         <v>84863480.480000094</v>
@@ -5440,7 +5559,7 @@
         <v>4241507</v>
       </c>
       <c r="I222">
-        <f>J222*3.5</f>
+        <f t="shared" si="2"/>
         <v>17.5</v>
       </c>
       <c r="J222">
@@ -5458,7 +5577,7 @@
         <v>43951</v>
       </c>
       <c r="B223" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C223">
         <v>89747591.620000005</v>
@@ -5467,7 +5586,7 @@
         <v>4241507</v>
       </c>
       <c r="I223">
-        <f>J223*3.5</f>
+        <f t="shared" si="2"/>
         <v>17.5</v>
       </c>
       <c r="J223">
@@ -5485,7 +5604,7 @@
         <v>43982</v>
       </c>
       <c r="B224" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C224">
         <v>103437574.34</v>
@@ -5494,7 +5613,7 @@
         <v>4241507</v>
       </c>
       <c r="I224">
-        <f>J224*3.5</f>
+        <f t="shared" si="2"/>
         <v>18.165000000000003</v>
       </c>
       <c r="J224">
@@ -5512,7 +5631,7 @@
         <v>44012</v>
       </c>
       <c r="B225" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C225">
         <v>100490240.53</v>
@@ -5521,7 +5640,7 @@
         <v>4241507</v>
       </c>
       <c r="I225">
-        <f>J225*3.5</f>
+        <f t="shared" si="2"/>
         <v>18.900000000000002</v>
       </c>
       <c r="J225">
@@ -5539,7 +5658,7 @@
         <v>44043</v>
       </c>
       <c r="B226" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C226">
         <v>106619102.02</v>
@@ -5548,7 +5667,7 @@
         <v>4241507</v>
       </c>
       <c r="I226">
-        <f>J226*3.5</f>
+        <f t="shared" si="2"/>
         <v>19.459999999999997</v>
       </c>
       <c r="J226">
@@ -5566,7 +5685,7 @@
         <v>44074</v>
       </c>
       <c r="B227" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C227">
         <v>103897664.94</v>
@@ -5575,7 +5694,7 @@
         <v>4241507</v>
       </c>
       <c r="I227">
-        <f>J227*3.5</f>
+        <f t="shared" si="2"/>
         <v>19.844999999999999</v>
       </c>
       <c r="J227">
@@ -5593,7 +5712,7 @@
         <v>44104</v>
       </c>
       <c r="B228" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C228">
         <v>97939284.209999993</v>
@@ -5602,7 +5721,7 @@
         <v>4241507</v>
       </c>
       <c r="I228">
-        <f>J228*3.5</f>
+        <f t="shared" si="2"/>
         <v>19.844999999999999</v>
       </c>
       <c r="J228">
@@ -5620,7 +5739,7 @@
         <v>44135</v>
       </c>
       <c r="B229" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C229">
         <v>99128982.030000001</v>
@@ -5629,7 +5748,7 @@
         <v>4241507</v>
       </c>
       <c r="I229">
-        <f>J229*3.5</f>
+        <f t="shared" si="2"/>
         <v>19.810000000000002</v>
       </c>
       <c r="J229">
@@ -5647,7 +5766,7 @@
         <v>44165</v>
       </c>
       <c r="B230" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C230">
         <v>89971220.120000005</v>
@@ -5656,7 +5775,7 @@
         <v>4241507</v>
       </c>
       <c r="I230">
-        <f>J230*3.5</f>
+        <f t="shared" si="2"/>
         <v>19.425000000000001</v>
       </c>
       <c r="J230">
@@ -5674,7 +5793,7 @@
         <v>44196</v>
       </c>
       <c r="B231" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C231">
         <v>96490032.159999996</v>
@@ -5683,7 +5802,7 @@
         <v>4241507</v>
       </c>
       <c r="I231">
-        <f>J231*3.5</f>
+        <f t="shared" si="2"/>
         <v>19.004999999999999</v>
       </c>
       <c r="J231">
@@ -5701,7 +5820,7 @@
         <v>44227</v>
       </c>
       <c r="B232" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C232">
         <v>100420129.45999999</v>
@@ -5710,7 +5829,7 @@
         <v>4246155</v>
       </c>
       <c r="I232">
-        <f>J232*3.5</f>
+        <f t="shared" si="2"/>
         <v>19.425000000000001</v>
       </c>
       <c r="J232">
@@ -5728,7 +5847,7 @@
         <v>44255</v>
       </c>
       <c r="B233" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C233">
         <v>88915911.659999907</v>
@@ -5737,7 +5856,7 @@
         <v>4246155</v>
       </c>
       <c r="I233">
-        <f>J233*3.5</f>
+        <f t="shared" ref="I233:I264" si="3">J233*3.5</f>
         <v>18.935000000000002</v>
       </c>
       <c r="J233">
@@ -5755,7 +5874,7 @@
         <v>44286</v>
       </c>
       <c r="B234" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C234">
         <v>109625158</v>
@@ -5764,7 +5883,7 @@
         <v>4246155</v>
       </c>
       <c r="I234">
-        <f>J234*3.5</f>
+        <f t="shared" si="3"/>
         <v>19.459999999999997</v>
       </c>
       <c r="J234">
@@ -5782,7 +5901,7 @@
         <v>44316</v>
       </c>
       <c r="B235" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C235">
         <v>110804219</v>
@@ -5791,7 +5910,7 @@
         <v>4246155</v>
       </c>
       <c r="I235">
-        <f>J235*3.5</f>
+        <f t="shared" si="3"/>
         <v>18.900000000000002</v>
       </c>
       <c r="J235">
@@ -5809,7 +5928,7 @@
         <v>44347</v>
       </c>
       <c r="B236" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C236">
         <v>105766531</v>
@@ -5818,7 +5937,7 @@
         <v>4246155</v>
       </c>
       <c r="I236">
-        <f>J236*3.5</f>
+        <f t="shared" si="3"/>
         <v>18.760000000000002</v>
       </c>
       <c r="J236">
@@ -5836,7 +5955,7 @@
         <v>44377</v>
       </c>
       <c r="B237" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C237">
         <v>99967034</v>
@@ -5845,7 +5964,7 @@
         <v>4246155</v>
       </c>
       <c r="I237">
-        <f>J237*3.5</f>
+        <f t="shared" si="3"/>
         <v>18.55</v>
       </c>
       <c r="J237">
@@ -5863,7 +5982,7 @@
         <v>44408</v>
       </c>
       <c r="B238" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C238">
         <v>103665072</v>
@@ -5872,7 +5991,7 @@
         <v>4246155</v>
       </c>
       <c r="I238">
-        <f>J238*3.5</f>
+        <f t="shared" si="3"/>
         <v>17.989999999999998</v>
       </c>
       <c r="J238">
@@ -5890,7 +6009,7 @@
         <v>44439</v>
       </c>
       <c r="B239" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C239">
         <v>100082323</v>
@@ -5899,7 +6018,7 @@
         <v>4246155</v>
       </c>
       <c r="I239">
-        <f>J239*3.5</f>
+        <f t="shared" si="3"/>
         <v>17.78</v>
       </c>
       <c r="J239">
@@ -5917,7 +6036,7 @@
         <v>44469</v>
       </c>
       <c r="B240" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C240">
         <v>95476203</v>
@@ -5926,7 +6045,7 @@
         <v>4246155</v>
       </c>
       <c r="I240">
-        <f>J240*3.5</f>
+        <f t="shared" si="3"/>
         <v>17.5</v>
       </c>
       <c r="J240">
@@ -5944,7 +6063,7 @@
         <v>44500</v>
       </c>
       <c r="B241" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C241">
         <v>93780372</v>
@@ -5953,7 +6072,7 @@
         <v>4246155</v>
       </c>
       <c r="I241">
-        <f>J241*3.5</f>
+        <f t="shared" si="3"/>
         <v>17.5</v>
       </c>
       <c r="J241">
@@ -5971,7 +6090,7 @@
         <v>44530</v>
       </c>
       <c r="B242" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C242">
         <v>86336104</v>
@@ -5980,7 +6099,7 @@
         <v>4246155</v>
       </c>
       <c r="I242">
-        <f>J242*3.5</f>
+        <f t="shared" si="3"/>
         <v>16.834999999999997</v>
       </c>
       <c r="J242">
@@ -5998,7 +6117,7 @@
         <v>43069</v>
       </c>
       <c r="B243" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C243">
         <v>77602861.950000018</v>
@@ -6018,7 +6137,7 @@
         <v>43100</v>
       </c>
       <c r="B244" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C244">
         <v>83766228.610000074</v>
@@ -6041,7 +6160,7 @@
         <v>43131</v>
       </c>
       <c r="B245" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C245">
         <v>77293130.299999967</v>
@@ -6064,7 +6183,7 @@
         <v>43159</v>
       </c>
       <c r="B246" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C246">
         <v>75851053.009999946</v>
@@ -6087,7 +6206,7 @@
         <v>43190</v>
       </c>
       <c r="B247" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C247">
         <v>85844883.749999925</v>
@@ -6110,7 +6229,7 @@
         <v>43220</v>
       </c>
       <c r="B248" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C248">
         <v>81509536.710000068</v>
@@ -6133,7 +6252,7 @@
         <v>43251</v>
       </c>
       <c r="B249" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C249">
         <v>83412645.749999911</v>
@@ -6156,7 +6275,7 @@
         <v>43281</v>
       </c>
       <c r="B250" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C250">
         <v>85213513.379999965</v>
@@ -6179,7 +6298,7 @@
         <v>43312</v>
       </c>
       <c r="B251" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C251">
         <v>87640211.699999958</v>
@@ -6202,7 +6321,7 @@
         <v>43343</v>
       </c>
       <c r="B252" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C252">
         <v>92079032.829999998</v>
@@ -6225,7 +6344,7 @@
         <v>43373</v>
       </c>
       <c r="B253" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C253">
         <v>86798408.920000017</v>
@@ -6248,7 +6367,7 @@
         <v>43404</v>
       </c>
       <c r="B254" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C254">
         <v>86864991.320000023</v>
@@ -6271,7 +6390,7 @@
         <v>43434</v>
       </c>
       <c r="B255" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C255">
         <v>85416660.939999968</v>
@@ -6294,7 +6413,7 @@
         <v>43465</v>
       </c>
       <c r="B256" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C256">
         <v>89259941.550000012</v>
@@ -6317,7 +6436,7 @@
         <v>43496</v>
       </c>
       <c r="B257" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C257">
         <v>84074108.510999933</v>
@@ -6340,7 +6459,7 @@
         <v>43524</v>
       </c>
       <c r="B258" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C258">
         <v>80159169.430000052</v>
@@ -6363,7 +6482,7 @@
         <v>43555</v>
       </c>
       <c r="B259" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C259">
         <v>90270817.340000123</v>
@@ -6386,7 +6505,7 @@
         <v>43585</v>
       </c>
       <c r="B260" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C260">
         <v>88258778.969999909</v>
@@ -6409,7 +6528,7 @@
         <v>43616</v>
       </c>
       <c r="B261" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C261">
         <v>89478821.050000012</v>
@@ -6432,7 +6551,7 @@
         <v>43646</v>
       </c>
       <c r="B262" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C262">
         <v>90820317.929999977</v>
@@ -6455,7 +6574,7 @@
         <v>43677</v>
       </c>
       <c r="B263" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C263">
         <v>97493520.25999999</v>
@@ -6478,7 +6597,7 @@
         <v>43708</v>
       </c>
       <c r="B264" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C264">
         <v>102984061.4799999</v>
@@ -6501,7 +6620,7 @@
         <v>43738</v>
       </c>
       <c r="B265" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C265">
         <v>95166188.089999944</v>
@@ -6524,7 +6643,7 @@
         <v>43769</v>
       </c>
       <c r="B266" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C266">
         <v>96419527.339999974</v>
@@ -6547,7 +6666,7 @@
         <v>43799</v>
       </c>
       <c r="B267" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C267">
         <v>96264380.500000164</v>
@@ -6570,7 +6689,7 @@
         <v>43830</v>
       </c>
       <c r="B268" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C268">
         <v>99226297.709999889</v>
@@ -6593,7 +6712,7 @@
         <v>43861</v>
       </c>
       <c r="B269" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C269">
         <v>96384145.400000021</v>
@@ -6616,7 +6735,7 @@
         <v>43890</v>
       </c>
       <c r="B270" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C270">
         <v>95018329.340000004</v>
@@ -6639,7 +6758,7 @@
         <v>43921</v>
       </c>
       <c r="B271" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C271">
         <v>115203393.43000001</v>
@@ -6662,7 +6781,7 @@
         <v>43951</v>
       </c>
       <c r="B272" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C272">
         <v>118514819.54000001</v>
@@ -6685,7 +6804,7 @@
         <v>43982</v>
       </c>
       <c r="B273" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C273">
         <v>130309611.09</v>
@@ -6708,7 +6827,7 @@
         <v>44012</v>
       </c>
       <c r="B274" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C274">
         <v>123418541.02</v>
@@ -6731,7 +6850,7 @@
         <v>44043</v>
       </c>
       <c r="B275" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C275">
         <v>130672533.3300001</v>
@@ -6754,7 +6873,7 @@
         <v>44074</v>
       </c>
       <c r="B276" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C276">
         <v>127341251.2400001</v>
@@ -6777,7 +6896,7 @@
         <v>44104</v>
       </c>
       <c r="B277" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C277">
         <v>123364376.20999999</v>
@@ -6800,7 +6919,7 @@
         <v>44135</v>
       </c>
       <c r="B278" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C278">
         <v>125577663.34</v>
@@ -6823,7 +6942,7 @@
         <v>44165</v>
       </c>
       <c r="B279" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C279">
         <v>117186979.63</v>
@@ -6846,7 +6965,7 @@
         <v>44196</v>
       </c>
       <c r="B280" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C280">
         <v>125751679.1699999</v>
@@ -6869,7 +6988,7 @@
         <v>44227</v>
       </c>
       <c r="B281" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C281">
         <v>125723145.94</v>
@@ -6892,7 +7011,7 @@
         <v>44255</v>
       </c>
       <c r="B282" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C282">
         <v>112387954.73</v>
@@ -6915,7 +7034,7 @@
         <v>44286</v>
       </c>
       <c r="B283" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C283">
         <v>132775073.5700001</v>
@@ -6938,7 +7057,7 @@
         <v>44316</v>
       </c>
       <c r="B284" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C284">
         <v>131672467.52</v>
@@ -6961,7 +7080,7 @@
         <v>44347</v>
       </c>
       <c r="B285" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C285">
         <v>127404814.09</v>
@@ -6984,7 +7103,7 @@
         <v>44377</v>
       </c>
       <c r="B286" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C286">
         <v>121468395.51000001</v>
@@ -7007,7 +7126,7 @@
         <v>44408</v>
       </c>
       <c r="B287" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C287">
         <v>127360947.56</v>
@@ -7030,7 +7149,7 @@
         <v>44439</v>
       </c>
       <c r="B288" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C288">
         <v>123196974.32999989</v>
@@ -7053,7 +7172,7 @@
         <v>44469</v>
       </c>
       <c r="B289" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C289">
         <v>117791496.17000011</v>
@@ -7076,7 +7195,7 @@
         <v>44500</v>
       </c>
       <c r="B290" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C290">
         <v>115931747.87</v>
@@ -7106,15 +7225,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEA8EF1-67C7-4898-9985-1A1D3954D610}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -7127,97 +7246,272 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
+        <v>42</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>12</v>
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>13</v>
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
+        <v>70</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>15</v>
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>16</v>
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
+        <v>46</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" t="s">
-        <v>38</v>
+        <v>52</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" t="s">
-        <v>42</v>
+        <v>50</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" t="s">
-        <v>44</v>
+        <v>47</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" t="s">
-        <v>46</v>
+        <v>51</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>48</v>
       </c>
+      <c r="B15" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B23">
+    <sortCondition ref="A2:A23"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="B17" r:id="rId1" xr:uid="{C10F81D1-BDFE-46FF-8621-DFC83BCE48D1}"/>
+    <hyperlink ref="B18" r:id="rId2" xr:uid="{4F3CA6F6-230A-4371-8D9C-43F435DFD434}"/>
+    <hyperlink ref="B20" r:id="rId3" xr:uid="{15AC42A4-D2B3-4B52-A1B7-297E825A26B1}"/>
+    <hyperlink ref="B16" r:id="rId4" xr:uid="{D882CFEF-D046-46E4-9D07-320E77AABCC1}"/>
+    <hyperlink ref="B19" r:id="rId5" xr:uid="{D724403B-2F47-4440-BEA3-AEDB80958022}"/>
+    <hyperlink ref="B9" r:id="rId6" xr:uid="{5F998710-1AE2-4A5B-B0DD-B3261A99594C}"/>
+    <hyperlink ref="B12" r:id="rId7" xr:uid="{4631FB91-5535-4655-87C7-2D445F11285E}"/>
+    <hyperlink ref="B15" r:id="rId8" xr:uid="{8B612440-5031-4374-8532-708FFF2F531C}"/>
+    <hyperlink ref="B14" r:id="rId9" xr:uid="{E428F5C6-169B-474B-8463-D3E01B6BE77A}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{C4A3B638-693E-4C8C-87D3-A62074CB2315}"/>
+    <hyperlink ref="B13" r:id="rId11" xr:uid="{1346D462-7FC0-4009-BC59-A67858E44437}"/>
+    <hyperlink ref="B10" r:id="rId12" xr:uid="{D7CC0C3E-2EBA-428F-A111-11C709C1E4B8}"/>
+    <hyperlink ref="B8" r:id="rId13" xr:uid="{81BBAA8B-F5BD-4203-A5CD-C21D327A0698}"/>
+    <hyperlink ref="B21" r:id="rId14" xr:uid="{AA0E4D10-7F89-43AD-AB60-6E62C3CC814F}"/>
+    <hyperlink ref="B3" r:id="rId15" xr:uid="{21F59278-D845-441B-99D1-A7038D0E6491}"/>
+    <hyperlink ref="B4" r:id="rId16" xr:uid="{51D72070-5265-4C99-BF22-F5EB56CD22A2}"/>
+    <hyperlink ref="B2" r:id="rId17" xr:uid="{56C1DAF7-0920-4C8B-9BE0-5C3CDCBCC943}"/>
+    <hyperlink ref="B5" r:id="rId18" xr:uid="{7603472C-2E0E-499E-A581-4E366844C695}"/>
+    <hyperlink ref="B7" r:id="rId19" xr:uid="{3363E57A-01C1-47D7-9561-8D47BE605D3F}"/>
+    <hyperlink ref="B6" r:id="rId20" xr:uid="{C9EA466C-8078-4693-A698-8D24A6D83E3B}"/>
+    <hyperlink ref="B22" r:id="rId21" xr:uid="{FF553C78-2C89-49C8-B3D7-CC4285DFE326}"/>
+    <hyperlink ref="B23" r:id="rId22" xr:uid="{D67EF7AF-3681-4707-9720-56A9C0DF1ED8}"/>
+    <hyperlink ref="B30" r:id="rId23" xr:uid="{6EF92AEE-E17F-4F77-B5EF-D1BE9398438C}"/>
+    <hyperlink ref="B24" r:id="rId24" xr:uid="{94A79736-0420-4BC6-910B-D5DBDBCCEAA5}"/>
+    <hyperlink ref="B25" r:id="rId25" xr:uid="{92A80099-CAF0-4233-938A-A4E99B439A0C}"/>
+    <hyperlink ref="B26" r:id="rId26" xr:uid="{994B2162-9E8A-4B3E-8789-28FE62509F6B}"/>
+    <hyperlink ref="B27" r:id="rId27" xr:uid="{51DE0D95-FACD-480F-9E6D-646A03F60A38}"/>
+    <hyperlink ref="B28" r:id="rId28" xr:uid="{B93557A7-7F5C-4969-85D5-68040B1DF818}"/>
+    <hyperlink ref="B29" r:id="rId29" xr:uid="{E09CFE9B-297A-44A2-B240-1CABABE97B21}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>